<commit_message>
Report Templating * Fix an error in the documentation for the project model related to project key photos
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom.kamin\Sitka Technology Group, Inc\Stewart Gordon - ProjectFirma Report Center Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="386" documentId="13_ncr:1_{6A3F707F-B1FD-4FAD-951D-97A69186F5E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C00B8392-2D93-49E9-9E4D-30E28B570638}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50A1E42-4537-4BE6-8FCC-190CC70FD764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23670" yWindow="5190" windowWidth="32445" windowHeight="21435" activeTab="6" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="5595" yWindow="3555" windowWidth="43200" windowHeight="23535" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="243">
   <si>
     <t>Description of Field</t>
   </si>
@@ -572,9 +572,6 @@
   </si>
   <si>
     <t>Get the Project Key Photo</t>
-  </si>
-  <si>
-    <t>&lt;% var projectKeyPhoto = project.GetKeyPhoto(); %&gt;</t>
   </si>
   <si>
     <t>Get all Project Images</t>
@@ -1543,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,61 +1902,61 @@
         <v>142</v>
       </c>
       <c r="D29" s="54" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="E29" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B30" s="57" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" s="54" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="54" t="s">
-        <v>145</v>
-      </c>
       <c r="E30" s="57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B31" s="57" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="57" t="s">
+        <v>200</v>
+      </c>
+      <c r="D31" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="D31" s="54" t="s">
+      <c r="E31" s="57" t="s">
         <v>202</v>
-      </c>
-      <c r="E31" s="57" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B32" s="57" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D32" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="57" t="s">
         <v>148</v>
-      </c>
-      <c r="E32" s="57" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2043,19 +2040,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2064,10 +2061,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E5" s="15"/>
     </row>
@@ -2077,10 +2074,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>154</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>155</v>
       </c>
       <c r="E6" s="15"/>
     </row>
@@ -2090,10 +2087,10 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E7" s="25"/>
     </row>
@@ -2101,10 +2098,10 @@
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E8" s="25"/>
     </row>
@@ -2112,10 +2109,10 @@
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" s="25"/>
     </row>
@@ -2123,39 +2120,39 @@
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="31" t="s">
         <v>183</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D11" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>185</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="31" t="s">
         <v>164</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2164,7 +2161,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>50</v>
@@ -2177,7 +2174,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>50</v>
@@ -2186,19 +2183,19 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="36" t="s">
         <v>167</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2207,10 +2204,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>169</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>170</v>
       </c>
       <c r="E16" s="38"/>
     </row>
@@ -2220,10 +2217,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E17" s="38"/>
     </row>
@@ -2233,10 +2230,10 @@
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E18" s="25"/>
     </row>
@@ -2244,10 +2241,10 @@
       <c r="A19" s="27"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E19" s="25"/>
     </row>
@@ -2255,10 +2252,10 @@
       <c r="A20" s="27"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E20" s="25"/>
     </row>
@@ -2266,39 +2263,39 @@
       <c r="A21" s="27"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2307,7 +2304,7 @@
         <v>48</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>50</v>
@@ -2320,7 +2317,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>50</v>
@@ -2338,10 +2335,10 @@
         <v>142</v>
       </c>
       <c r="D26" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>177</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2350,10 +2347,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E27" s="15"/>
     </row>
@@ -2363,10 +2360,10 @@
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="25"/>
     </row>
@@ -2374,10 +2371,10 @@
       <c r="A29" s="27"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E29" s="25"/>
     </row>
@@ -2385,10 +2382,10 @@
       <c r="A30" s="27"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E30" s="25"/>
     </row>
@@ -2396,26 +2393,26 @@
       <c r="A31" s="27"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2424,7 +2421,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>50</v>
@@ -2790,7 +2787,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24" t="s">
@@ -3388,7 +3385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9A00D5-E39F-4947-BF8A-C9BC6B110727}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3446,19 +3443,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>204</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3467,10 +3464,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E5" s="13"/>
     </row>
@@ -3480,75 +3477,75 @@
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>208</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>209</v>
       </c>
       <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>218</v>
-      </c>
       <c r="E9" s="58" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D10" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" s="58" t="s">
         <v>221</v>
-      </c>
-      <c r="E10" s="58" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E11" s="59"/>
     </row>
@@ -3556,10 +3553,10 @@
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>226</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>227</v>
       </c>
       <c r="E12" s="59"/>
     </row>
@@ -3567,78 +3564,78 @@
       <c r="A13" s="27"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E13" s="59" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="24"/>
       <c r="C14" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E15" s="59" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E17" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="24"/>
       <c r="C18" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D18" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E18" s="59" t="s">
         <v>236</v>
-      </c>
-      <c r="E18" s="59" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3647,7 +3644,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
PF-2292 Idaho: Extend report center model to support Reported PMs and Engr & Tech Asst data * Updating documentation with the new models added * Minor refactoring of names to make consistent with rest of models
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50A1E42-4537-4BE6-8FCC-190CC70FD764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5459434A-6688-4191-8C9F-DA42716DF2A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="3555" windowWidth="43200" windowHeight="23535" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="9" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Person" sheetId="2" r:id="rId5"/>
     <sheet name="Organization" sheetId="3" r:id="rId6"/>
     <sheet name="ProjectStatus" sheetId="7" r:id="rId7"/>
+    <sheet name="ReportedPerformanceMeasure" sheetId="8" r:id="rId8"/>
+    <sheet name="ExpectedPerformanceMeasure" sheetId="9" r:id="rId9"/>
+    <sheet name="TechnicalAssistanceRequest" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="321">
   <si>
     <t>Description of Field</t>
   </si>
@@ -948,12 +951,334 @@
   <si>
     <t>*Project Status Risks Or Issues</t>
   </si>
+  <si>
+    <t>Get All Project Reported Performance Measure Values</t>
+  </si>
+  <si>
+    <t>&lt;% if(reportedPerformanceMeasures.Any()) { ?&gt;</t>
+  </si>
+  <si>
+    <t>If there are Reported Performance Measure Values</t>
+  </si>
+  <si>
+    <t>&lt;% foreach(var reportedPerformanceMeasure in reportedPerformanceMeasures) { %&gt;</t>
+  </si>
+  <si>
+    <t>End the Reported Performance Measure Value loop</t>
+  </si>
+  <si>
+    <t>Performance Measure Name</t>
+  </si>
+  <si>
+    <t>Performance Measure Subcategory Name</t>
+  </si>
+  <si>
+    <t>Performance Measure Subcategory Option Name</t>
+  </si>
+  <si>
+    <t>The Value of the Reported Performance Measure</t>
+  </si>
+  <si>
+    <t>The Year of the Reported Performance Measure</t>
+  </si>
+  <si>
+    <t>The Unit Type of the Reported Performance Measure</t>
+  </si>
+  <si>
+    <t>&lt;%= reportedPerformanceMeasure.PerformanceMeasureName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= reportedPerformanceMeasure.PerformanceMeasureSubcategoryName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= reportedPerformanceMeasure.PerformanceMeasureSubcategoryOptionName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= reportedPerformanceMeasure.Value %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= reportedPerformanceMeasure.UnitType %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= reportedPerformanceMeasure.Year %&gt;</t>
+  </si>
+  <si>
+    <t>Returns a list of ProjectReportedPerformanceMeasure models</t>
+  </si>
+  <si>
+    <t>&lt;%= var reportedPerformanceMeasures = project.GetProjectReportedPerformanceMeasures(); %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= var expectedPerformanceMeasures = project.GetProjectExpectedPerformanceMeasures(); %&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns a list of ProjectReportedPerformanceMeasure models (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ReportedPerformanceMeasure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns a list of ProjectExpectedPerformanceMeasure models (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ExpectedPerformanceMeasure </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tab)</t>
+    </r>
+  </si>
+  <si>
+    <t>ProjectReportedPerformanceMeasure</t>
+  </si>
+  <si>
+    <t>Start Reported Performance Measure Value loop</t>
+  </si>
+  <si>
+    <t>Get All Project Expected Performance Measure Values</t>
+  </si>
+  <si>
+    <t>Returns a list of ProjectExpectedPerformanceMeasure models</t>
+  </si>
+  <si>
+    <t>If there are Expected Performance Measure Values</t>
+  </si>
+  <si>
+    <t>Start Expected Performance Measure Value loop</t>
+  </si>
+  <si>
+    <t>ProjectExpectedPerformanceMeasure</t>
+  </si>
+  <si>
+    <t>The Value of the Expected Performance Measure</t>
+  </si>
+  <si>
+    <t>The Unit Type of the Expected Performance Measure</t>
+  </si>
+  <si>
+    <t>End the Expected Performance Measure Value loop</t>
+  </si>
+  <si>
+    <t>&lt;% if(expectedPerformanceMeasures.Any()) { ?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% foreach(var expectedPerformanceMeasure in expectedPerformanceMeasures) { %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= expectedPerformanceMeasure.PerformanceMeasureName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= expectedPerformanceMeasure.PerformanceMeasureSubcategoryName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= expectedPerformanceMeasure.PerformanceMeasureSubcategoryOptionName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= expectedPerformanceMeasure.Value %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= expectedPerformanceMeasure.UnitType %&gt;</t>
+  </si>
+  <si>
+    <t>ProjectReportedPerformanceMeasure(s)</t>
+  </si>
+  <si>
+    <t>ProjectExpectedPerformanceMeasure(s)</t>
+  </si>
+  <si>
+    <t>Get all Project Technical Assistance Requests</t>
+  </si>
+  <si>
+    <t>Get All Project Expected Performance Measure values</t>
+  </si>
+  <si>
+    <t>Tenant Specificity</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>ISWCC Only</t>
+  </si>
+  <si>
+    <t>&lt;%= var technicalAssistanceRequests = project.GetProjectTechnicalAssistanceRequests(); %&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns a list of ProjectTechnicalAssistanceRequest models (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>TechnicalAssistanceRequest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tab)</t>
+    </r>
+  </si>
+  <si>
+    <t>ProjectTechnicalAssistanceRequest(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This model is only applicable to ISWCC's ProjectFirma Instance. </t>
+  </si>
+  <si>
+    <t>ProjectTechnicalAssistanceRequest</t>
+  </si>
+  <si>
+    <t>If there are Project Technical Assistance Requests</t>
+  </si>
+  <si>
+    <t>Start Project Technical Assistance Requests loop</t>
+  </si>
+  <si>
+    <t>Assigned Person</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Hours Requested</t>
+  </si>
+  <si>
+    <t>Hours Allocated</t>
+  </si>
+  <si>
+    <t>Hours Provided</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Dollar Value Decimal Value</t>
+  </si>
+  <si>
+    <t>Dollar Value String (text) Value</t>
+  </si>
+  <si>
+    <t>Returns a list of ProjectTechnicalAssistanceRequest models</t>
+  </si>
+  <si>
+    <t>&lt;% if(technicalAssistanceRequests.Any()) { ?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% foreach(var technicalAssistanceRequest in technicalAssistanceRequests) { %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= technicalAssistanceRequest.FiscalYear %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= technicalAssistanceRequest.Notes %&gt;</t>
+  </si>
+  <si>
+    <t>Fiscal Year</t>
+  </si>
+  <si>
+    <t>&lt;%= technicalAssistanceRequest.Type %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= technicalAssistanceRequest.HoursRequested %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= technicalAssistanceRequest.HoursAllocated %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= technicalAssistanceRequest.HoursPrivded %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= technicalAssistanceRequest.DollarValueDecimal %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= technicalAssistanceRequest.DollarValueString %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% var assignedPerson =  technicalAssistanceRequest.AssignedPerson; %&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns a single Person model (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Person</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tab)</t>
+    </r>
+  </si>
+  <si>
+    <t>Returns the raw decimal value (e.g. 10.05) useful for adding/calculations</t>
+  </si>
+  <si>
+    <t>Returns a dollar formatted text value (e.g. $10.05) useful for simply displaying dollar value</t>
+  </si>
+  <si>
+    <t>End the Project Technical Assistance Requests loop</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1045,8 +1370,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1143,6 +1491,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1153,11 +1506,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1211,7 +1565,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1223,8 +1576,12 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FB0E11C-9AD4-467E-ABE3-B008EF9DCF04}"/>
   </cellStyles>
@@ -1538,22 +1895,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="69.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" customWidth="1"/>
+    <col min="5" max="5" width="100.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1567,8 +1925,11 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>134</v>
       </c>
@@ -1580,8 +1941,9 @@
         <v>136</v>
       </c>
       <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>9</v>
       </c>
@@ -1597,8 +1959,9 @@
       <c r="E3" s="47" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="47" t="s">
         <v>12</v>
@@ -1610,371 +1973,782 @@
         <v>13</v>
       </c>
       <c r="E4" s="47"/>
-    </row>
-    <row r="5" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53" t="s">
+      <c r="F4" s="47"/>
+    </row>
+    <row r="5" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="53"/>
-    </row>
-    <row r="6" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53" t="s">
+      <c r="E5" s="52"/>
+      <c r="F5" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53" t="s">
+      <c r="E6" s="52"/>
+      <c r="F6" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="53"/>
-    </row>
-    <row r="8" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53" t="s">
+      <c r="E7" s="52"/>
+      <c r="F7" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="53"/>
-    </row>
-    <row r="9" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53" t="s">
+      <c r="E8" s="52"/>
+      <c r="F8" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="53"/>
-    </row>
-    <row r="10" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53" t="s">
+      <c r="E9" s="52"/>
+      <c r="F9" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="53"/>
-    </row>
-    <row r="11" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53" t="s">
+      <c r="E10" s="52"/>
+      <c r="F10" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="53"/>
-    </row>
-    <row r="12" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53" t="s">
+      <c r="E11" s="52"/>
+      <c r="F11" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="53"/>
-    </row>
-    <row r="13" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53" t="s">
+      <c r="E12" s="52"/>
+      <c r="F12" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="53"/>
-    </row>
-    <row r="14" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53" t="s">
+      <c r="E13" s="52"/>
+      <c r="F13" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="53"/>
-    </row>
-    <row r="15" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53" t="s">
+      <c r="E14" s="52"/>
+      <c r="F14" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="53"/>
-    </row>
-    <row r="16" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53" t="s">
+      <c r="E15" s="52"/>
+      <c r="F15" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="53" t="s">
+      <c r="D16" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="53"/>
-    </row>
-    <row r="17" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53" t="s">
+      <c r="E16" s="52"/>
+      <c r="F16" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="53"/>
-    </row>
-    <row r="18" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53" t="s">
+      <c r="E17" s="52"/>
+      <c r="F17" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="53"/>
-    </row>
-    <row r="19" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53" t="s">
+      <c r="E18" s="52"/>
+      <c r="F18" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="53" t="s">
+      <c r="D19" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="53"/>
-    </row>
-    <row r="20" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53" t="s">
+      <c r="E19" s="52"/>
+      <c r="F19" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="53"/>
-    </row>
-    <row r="21" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53" t="s">
+      <c r="E20" s="52"/>
+      <c r="F20" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="53"/>
-    </row>
-    <row r="22" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53" t="s">
+      <c r="E21" s="52"/>
+      <c r="F21" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="53" t="s">
+      <c r="D22" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="E22" s="53"/>
-    </row>
-    <row r="23" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53" t="s">
+      <c r="E22" s="52"/>
+      <c r="F22" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="52"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D23" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="E23" s="53"/>
-    </row>
-    <row r="24" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53" t="s">
+      <c r="E23" s="52"/>
+      <c r="F23" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="53"/>
-    </row>
-    <row r="25" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53" t="s">
+      <c r="E24" s="52"/>
+      <c r="F24" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="52"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="52" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53" t="s">
+      <c r="F25" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="D26" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="53" t="s">
+      <c r="E26" s="52" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+      <c r="F26" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>282</v>
+      </c>
+      <c r="B27" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>261</v>
+      </c>
+      <c r="E27" s="52" t="s">
+        <v>263</v>
+      </c>
+      <c r="F27" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>285</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="F28" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B29" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C29" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D29" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E29" s="53" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="55" t="s">
+      <c r="F29" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="56" t="s">
+      <c r="B30" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C30" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D30" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E30" s="56" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="55" t="s">
+      <c r="F30" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C31" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="D29" s="54" t="s">
+      <c r="D31" s="53" t="s">
         <v>176</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E31" s="56" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+      <c r="F31" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B32" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C32" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="D30" s="54" t="s">
+      <c r="D32" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E32" s="56" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="55" t="s">
+      <c r="F32" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B33" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C33" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="D31" s="54" t="s">
+      <c r="D33" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="E31" s="57" t="s">
+      <c r="E33" s="56" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="55" t="s">
+      <c r="F33" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="57" t="s">
+      <c r="B34" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="57" t="s">
+      <c r="C34" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D34" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E34" s="56" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
-      <c r="B33" s="48" t="s">
+      <c r="F34" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="54" t="s">
+        <v>291</v>
+      </c>
+      <c r="B35" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="56" t="s">
+        <v>284</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>289</v>
+      </c>
+      <c r="E35" s="56" t="s">
+        <v>290</v>
+      </c>
+      <c r="F35" s="60" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="48"/>
+      <c r="B36" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C36" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="48" t="s">
+      <c r="D36" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CD1C35-1AF3-403F-B823-0BA284571615}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="72" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+    </row>
+    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="42"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="54" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2451,7 +3225,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,17 +3426,17 @@
       <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="49"/>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
@@ -2715,7 +3489,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -2730,7 +3504,7 @@
       <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
       </c>
@@ -2740,7 +3514,7 @@
       <c r="D3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="52"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -2893,7 +3667,7 @@
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="43" t="s">
         <v>48</v>
       </c>
@@ -2903,7 +3677,7 @@
       <c r="D16" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="52"/>
+      <c r="E16" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3414,7 +4188,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -3429,7 +4203,7 @@
       <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
       </c>
@@ -3439,7 +4213,7 @@
       <c r="D3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="52"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -3495,7 +4269,7 @@
       <c r="D7" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="57" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3508,7 +4282,7 @@
       <c r="D8" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="57" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3521,7 +4295,7 @@
       <c r="D9" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="57" t="s">
         <v>219</v>
       </c>
     </row>
@@ -3534,7 +4308,7 @@
       <c r="D10" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="57" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3547,7 +4321,7 @@
       <c r="D11" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="E11" s="59"/>
+      <c r="E11" s="58"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
@@ -3558,7 +4332,7 @@
       <c r="D12" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="E12" s="59"/>
+      <c r="E12" s="58"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
@@ -3569,7 +4343,7 @@
       <c r="D13" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="58" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3582,7 +4356,7 @@
       <c r="D14" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="58" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3595,7 +4369,7 @@
       <c r="D15" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="58" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3608,7 +4382,7 @@
       <c r="D16" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="58" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3621,7 +4395,7 @@
       <c r="D17" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="58" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3634,7 +4408,7 @@
       <c r="D18" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="58" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3649,7 +4423,7 @@
       <c r="D19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="60"/>
+      <c r="E19" s="59"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
@@ -3660,10 +4434,10 @@
       <c r="D20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="60"/>
+      <c r="E20" s="59"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="43" t="s">
         <v>48</v>
       </c>
@@ -3673,10 +4447,433 @@
       <c r="D21" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="52"/>
+      <c r="E21" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345078EF-4E02-4B0D-B586-01D7A19E1A69}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F62140-8660-4506-8649-E7BD6D8F000F}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PF-2292 Idaho: Extend report center model to support Reported PMs and Engr & Tech Asst data * adding comments to expected pm worksheet
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5459434A-6688-4191-8C9F-DA42716DF2A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31DB2A3-DD92-4B74-9BB8-927BFF7AF405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="9" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="8" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="323">
   <si>
     <t>Description of Field</t>
   </si>
@@ -1272,6 +1272,12 @@
   </si>
   <si>
     <t>End the Project Technical Assistance Requests loop</t>
+  </si>
+  <si>
+    <t>Entering subcategory information is optional for Expected Performance Measures, so this may return null</t>
+  </si>
+  <si>
+    <t>Entering values is optional for Expected Performance Measures, so this may return null</t>
   </si>
 </sst>
 </file>
@@ -2491,7 +2497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CD1C35-1AF3-403F-B823-0BA284571615}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -4676,8 +4682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F62140-8660-4506-8649-E7BD6D8F000F}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4686,7 +4692,7 @@
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="50.5703125" customWidth="1"/>
     <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="5" max="5" width="84.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4810,7 +4816,9 @@
       <c r="D9" s="24" t="s">
         <v>279</v>
       </c>
-      <c r="E9" s="28"/>
+      <c r="E9" s="28" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
@@ -4821,7 +4829,9 @@
       <c r="D10" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="57" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
@@ -4875,5 +4885,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PF-2292 Idaho: Extend report center model to support Reported PMs and Engr & Tech Asst data * change ISWCC to Idaho Soil & Water Conservation Commission
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31DB2A3-DD92-4B74-9BB8-927BFF7AF405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681FDE07-F721-4935-B778-164BB462F555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="8" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="9" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1133,9 +1133,6 @@
     <t>All</t>
   </si>
   <si>
-    <t>ISWCC Only</t>
-  </si>
-  <si>
     <t>&lt;%= var technicalAssistanceRequests = project.GetProjectTechnicalAssistanceRequests(); %&gt;</t>
   </si>
   <si>
@@ -1166,9 +1163,6 @@
     <t>ProjectTechnicalAssistanceRequest(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">This model is only applicable to ISWCC's ProjectFirma Instance. </t>
-  </si>
-  <si>
     <t>ProjectTechnicalAssistanceRequest</t>
   </si>
   <si>
@@ -1278,6 +1272,12 @@
   </si>
   <si>
     <t>Entering values is optional for Expected Performance Measures, so this may return null</t>
+  </si>
+  <si>
+    <t>Idaho Soil &amp; Water Conservation Commission Only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: This model is only applicable to Idaho Soil &amp; Water Conservation Commission's ProjectFirma Instance. </t>
   </si>
 </sst>
 </file>
@@ -1904,7 +1904,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,7 +1914,7 @@
     <col min="3" max="3" width="45.85546875" customWidth="1"/>
     <col min="4" max="4" width="77.85546875" customWidth="1"/>
     <col min="5" max="5" width="100.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
     </row>
     <row r="35" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="54" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B35" s="56" t="s">
         <v>5</v>
@@ -2464,13 +2464,13 @@
         <v>284</v>
       </c>
       <c r="D35" s="52" t="s">
+        <v>288</v>
+      </c>
+      <c r="E35" s="56" t="s">
         <v>289</v>
       </c>
-      <c r="E35" s="56" t="s">
-        <v>290</v>
-      </c>
       <c r="F35" s="60" t="s">
-        <v>288</v>
+        <v>321</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2497,8 +2497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CD1C35-1AF3-403F-B823-0BA284571615}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,7 +2512,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
-        <v>292</v>
+        <v>322</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>5</v>
@@ -2575,10 +2575,10 @@
         <v>284</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2587,10 +2587,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E6" s="15"/>
     </row>
@@ -2600,23 +2600,23 @@
         <v>12</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E8" s="25"/>
     </row>
@@ -2624,23 +2624,23 @@
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E10" s="28"/>
     </row>
@@ -2648,10 +2648,10 @@
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E11" s="29"/>
     </row>
@@ -2659,10 +2659,10 @@
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E12" s="25"/>
     </row>
@@ -2670,10 +2670,10 @@
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E13" s="25"/>
     </row>
@@ -2681,10 +2681,10 @@
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E14" s="25"/>
     </row>
@@ -2692,26 +2692,26 @@
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2720,7 +2720,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>50</v>
@@ -4682,7 +4682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F62140-8660-4506-8649-E7BD6D8F000F}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -4817,7 +4817,7 @@
         <v>279</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4830,7 +4830,7 @@
         <v>280</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
PF-2292 Idaho: Extend report center model to support Reported PMs and Engr & Tech Asst data * editing expected pm tab to say return empty string instead of null * filtering out "Default" values * ordering reports on projects list
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681FDE07-F721-4935-B778-164BB462F555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C619BF68-8429-4371-AC1F-5349D8788985}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="9" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="7" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1268,16 +1268,16 @@
     <t>End the Project Technical Assistance Requests loop</t>
   </si>
   <si>
-    <t>Entering subcategory information is optional for Expected Performance Measures, so this may return null</t>
-  </si>
-  <si>
-    <t>Entering values is optional for Expected Performance Measures, so this may return null</t>
-  </si>
-  <si>
     <t>Idaho Soil &amp; Water Conservation Commission Only</t>
   </si>
   <si>
     <t xml:space="preserve">NOTE: This model is only applicable to Idaho Soil &amp; Water Conservation Commission's ProjectFirma Instance. </t>
+  </si>
+  <si>
+    <t>Entering subcategory information is optional for Expected Performance Measures, so this may return an empty string</t>
+  </si>
+  <si>
+    <t>Entering values is optional for Expected Performance Measures, so this may return an empty string</t>
   </si>
 </sst>
 </file>
@@ -2470,7 +2470,7 @@
         <v>289</v>
       </c>
       <c r="F35" s="60" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2497,7 +2497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CD1C35-1AF3-403F-B823-0BA284571615}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -2512,7 +2512,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -4465,8 +4465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345078EF-4E02-4B0D-B586-01D7A19E1A69}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4683,7 +4683,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4692,7 +4692,7 @@
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="50.5703125" customWidth="1"/>
     <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="84.140625" customWidth="1"/>
+    <col min="5" max="5" width="92.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4817,7 +4817,7 @@
         <v>279</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4830,7 +4830,7 @@
         <v>280</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
PF-2620: Added expenditures to project model. Added decimal representation for total estimated cost and expenditure so CA RCDs can roll up budget/expenditures in reports. Pork: removed reference to technical assistance from the ProjectFirma-Reports-Model-Documentation.xlsx
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/Training/ProjectFirma-Reports-Model-Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shannon.bulloch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C619BF68-8429-4371-AC1F-5349D8788985}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FAAA4E-A6EE-4BC5-A685-3B21A5E46F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="7" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="ProjectStatus" sheetId="7" r:id="rId7"/>
     <sheet name="ReportedPerformanceMeasure" sheetId="8" r:id="rId8"/>
     <sheet name="ExpectedPerformanceMeasure" sheetId="9" r:id="rId9"/>
-    <sheet name="TechnicalAssistanceRequest" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="297">
   <si>
     <t>Description of Field</t>
   </si>
@@ -1121,9 +1120,6 @@
     <t>ProjectExpectedPerformanceMeasure(s)</t>
   </si>
   <si>
-    <t>Get all Project Technical Assistance Requests</t>
-  </si>
-  <si>
     <t>Get All Project Expected Performance Measure values</t>
   </si>
   <si>
@@ -1133,158 +1129,41 @@
     <t>All</t>
   </si>
   <si>
-    <t>&lt;%= var technicalAssistanceRequests = project.GetProjectTechnicalAssistanceRequests(); %&gt;</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Returns a list of ProjectTechnicalAssistanceRequest models (see </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>TechnicalAssistanceRequest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tab)</t>
-    </r>
-  </si>
-  <si>
-    <t>ProjectTechnicalAssistanceRequest(s)</t>
-  </si>
-  <si>
-    <t>ProjectTechnicalAssistanceRequest</t>
-  </si>
-  <si>
-    <t>If there are Project Technical Assistance Requests</t>
-  </si>
-  <si>
-    <t>Start Project Technical Assistance Requests loop</t>
-  </si>
-  <si>
-    <t>Assigned Person</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Hours Requested</t>
-  </si>
-  <si>
-    <t>Hours Allocated</t>
-  </si>
-  <si>
-    <t>Hours Provided</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Dollar Value Decimal Value</t>
-  </si>
-  <si>
-    <t>Dollar Value String (text) Value</t>
-  </si>
-  <si>
-    <t>Returns a list of ProjectTechnicalAssistanceRequest models</t>
-  </si>
-  <si>
-    <t>&lt;% if(technicalAssistanceRequests.Any()) { ?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;% foreach(var technicalAssistanceRequest in technicalAssistanceRequests) { %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.FiscalYear %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.Notes %&gt;</t>
-  </si>
-  <si>
-    <t>Fiscal Year</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.Type %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.HoursRequested %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.HoursAllocated %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.HoursPrivded %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.DollarValueDecimal %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.DollarValueString %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;% var assignedPerson =  technicalAssistanceRequest.AssignedPerson; %&gt;</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Returns a single Person model (see </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Person</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tab)</t>
-    </r>
-  </si>
-  <si>
-    <t>Returns the raw decimal value (e.g. 10.05) useful for adding/calculations</t>
-  </si>
-  <si>
-    <t>Returns a dollar formatted text value (e.g. $10.05) useful for simply displaying dollar value</t>
-  </si>
-  <si>
-    <t>End the Project Technical Assistance Requests loop</t>
-  </si>
-  <si>
-    <t>Idaho Soil &amp; Water Conservation Commission Only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE: This model is only applicable to Idaho Soil &amp; Water Conservation Commission's ProjectFirma Instance. </t>
-  </si>
-  <si>
     <t>Entering subcategory information is optional for Expected Performance Measures, so this may return an empty string</t>
   </si>
   <si>
     <t>Entering values is optional for Expected Performance Measures, so this may return an empty string</t>
+  </si>
+  <si>
+    <t>&lt;%= project.EstimatedTotalCostDecimal %&gt;</t>
+  </si>
+  <si>
+    <t>Total Expenditures</t>
+  </si>
+  <si>
+    <t>Estimated Total Cost Decimal</t>
+  </si>
+  <si>
+    <t>Total Expenditures Decimal</t>
+  </si>
+  <si>
+    <t>&lt;%= project.TotalExpenditures %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= project.TotalExpendituresDecimal %&gt;</t>
+  </si>
+  <si>
+    <t>decimal value that can be used in aggregate functions (e.g. sum of expenditures for all projects)</t>
+  </si>
+  <si>
+    <t>decimal value that can be used in aggregate functions (e.g. sum of budget for all projects)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1377,13 +1256,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1391,16 +1263,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1497,11 +1361,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1512,82 +1371,76 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FB0E11C-9AD4-467E-ABE3-B008EF9DCF04}"/>
   </cellStyles>
@@ -1901,23 +1754,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" customWidth="1"/>
-    <col min="5" max="5" width="100.5703125" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="77.88671875" customWidth="1"/>
+    <col min="5" max="5" width="100.5546875" customWidth="1"/>
+    <col min="6" max="6" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1932,10 +1783,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="45" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>134</v>
       </c>
@@ -1949,812 +1800,573 @@
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="47"/>
-    </row>
-    <row r="4" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47" t="s">
+      <c r="F3" s="46"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-    </row>
-    <row r="5" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52" t="s">
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52" t="s">
+      <c r="E5" s="51"/>
+      <c r="F5" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52" t="s">
+      <c r="E6" s="51"/>
+      <c r="F6" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52" t="s">
+      <c r="E7" s="51"/>
+      <c r="F7" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52" t="s">
+      <c r="E8" s="51"/>
+      <c r="F8" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52" t="s">
+      <c r="E9" s="51"/>
+      <c r="F9" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52" t="s">
+      <c r="E10" s="51"/>
+      <c r="F10" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52" t="s">
+      <c r="E11" s="51"/>
+      <c r="F11" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52" t="s">
+      <c r="E12" s="51"/>
+      <c r="F12" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52" t="s">
+      <c r="E13" s="51"/>
+      <c r="F13" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52" t="s">
+      <c r="E14" s="51"/>
+      <c r="F14" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52" t="s">
+      <c r="E15" s="51"/>
+      <c r="F15" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="52" t="s">
+      <c r="D16" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52" t="s">
+      <c r="E16" s="51"/>
+      <c r="F16" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52" t="s">
+      <c r="E17" s="51"/>
+      <c r="F17" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52" t="s">
+      <c r="E18" s="51"/>
+      <c r="F18" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52" t="s">
+      <c r="E19" s="51"/>
+      <c r="F19" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="51"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51" t="s">
+        <v>291</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>289</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>296</v>
+      </c>
+      <c r="F20" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51" t="s">
+        <v>290</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="51"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51" t="s">
+        <v>292</v>
+      </c>
+      <c r="D22" s="51" t="s">
+        <v>294</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="F22" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="51"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="52" t="s">
+      <c r="D23" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52" t="s">
+      <c r="E23" s="51"/>
+      <c r="F23" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="51"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="52" t="s">
+      <c r="D24" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52" t="s">
+      <c r="E24" s="51"/>
+      <c r="F24" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="51"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D25" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52" t="s">
+      <c r="E25" s="51"/>
+      <c r="F25" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="52" t="s">
+      <c r="D26" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52" t="s">
+      <c r="E26" s="51"/>
+      <c r="F26" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="51"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="52" t="s">
+      <c r="D27" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52" t="s">
+      <c r="E27" s="51"/>
+      <c r="F27" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="51"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="52" t="s">
+      <c r="D28" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="52" t="s">
+      <c r="E28" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52" t="s">
+      <c r="F28" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="51"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D29" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="52" t="s">
+      <c r="E29" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
+      <c r="F29" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="51" t="s">
         <v>282</v>
       </c>
-      <c r="B27" s="52" t="s">
+      <c r="B30" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C30" s="51" t="s">
         <v>243</v>
       </c>
-      <c r="D27" s="52" t="s">
+      <c r="D30" s="51" t="s">
         <v>261</v>
       </c>
-      <c r="E27" s="52" t="s">
+      <c r="E30" s="51" t="s">
         <v>263</v>
       </c>
-      <c r="F27" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
+      <c r="F30" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="51" t="s">
         <v>283</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B31" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="52" t="s">
-        <v>285</v>
-      </c>
-      <c r="D28" s="52" t="s">
+      <c r="C31" s="51" t="s">
+        <v>284</v>
+      </c>
+      <c r="D31" s="51" t="s">
         <v>262</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="E31" s="51" t="s">
         <v>264</v>
       </c>
-      <c r="F28" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52" t="s">
+      <c r="F31" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="52" t="s">
+      <c r="B32" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="52" t="s">
+      <c r="C32" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="D32" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="53" t="s">
+      <c r="E32" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="F29" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
+      <c r="F32" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B33" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C33" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="53" t="s">
+      <c r="D33" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="56" t="s">
+      <c r="E33" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="F30" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
+      <c r="F33" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B34" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C34" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="D31" s="53" t="s">
+      <c r="D34" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E34" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="F31" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
+      <c r="F34" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B35" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C35" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="53" t="s">
+      <c r="D35" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E35" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="F32" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
+      <c r="F35" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="53" t="s">
         <v>199</v>
       </c>
-      <c r="B33" s="56" t="s">
+      <c r="B36" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C36" s="55" t="s">
         <v>200</v>
       </c>
-      <c r="D33" s="53" t="s">
+      <c r="D36" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="E33" s="56" t="s">
+      <c r="E36" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="F33" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
+      <c r="F36" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="56" t="s">
+      <c r="B37" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C37" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="D34" s="53" t="s">
+      <c r="D37" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="E34" s="56" t="s">
+      <c r="E37" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="F34" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
-        <v>290</v>
-      </c>
-      <c r="B35" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="56" t="s">
-        <v>284</v>
-      </c>
-      <c r="D35" s="52" t="s">
-        <v>288</v>
-      </c>
-      <c r="E35" s="56" t="s">
-        <v>289</v>
-      </c>
-      <c r="F35" s="60" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
-      <c r="B36" s="48" t="s">
+      <c r="F37" s="51" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="47"/>
+      <c r="B38" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C38" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="48" t="s">
+      <c r="D38" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CD1C35-1AF3-403F-B823-0BA284571615}">
-  <dimension ref="A1:E19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="72" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>320</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-    </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="42"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
-        <v>291</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24" t="s">
-        <v>307</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="E10" s="28"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24" t="s">
-        <v>296</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="E11" s="29"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>310</v>
-      </c>
-      <c r="E12" s="25"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24" t="s">
-        <v>298</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="E13" s="25"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="E14" s="25"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24" t="s">
-        <v>301</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>313</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="44"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2766,16 +2378,16 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2790,7 +2402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +2417,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2818,7 +2430,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>165</v>
       </c>
@@ -2835,7 +2447,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -2848,7 +2460,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -2861,7 +2473,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>141</v>
       </c>
@@ -2874,7 +2486,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -2885,7 +2497,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -2896,7 +2508,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -2909,7 +2521,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -2922,7 +2534,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -2935,7 +2547,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>48</v>
@@ -2948,7 +2560,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -2961,7 +2573,7 @@
       </c>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>165</v>
       </c>
@@ -2978,7 +2590,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
       <c r="B16" s="33" t="s">
         <v>6</v>
@@ -2991,7 +2603,7 @@
       </c>
       <c r="E16" s="38"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="37"/>
       <c r="B17" s="33" t="s">
         <v>12</v>
@@ -3004,7 +2616,7 @@
       </c>
       <c r="E17" s="38"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>141</v>
       </c>
@@ -3017,7 +2629,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="27"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
@@ -3028,7 +2640,7 @@
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
@@ -3039,7 +2651,7 @@
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
@@ -3052,7 +2664,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
@@ -3065,7 +2677,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
@@ -3078,7 +2690,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
       <c r="B24" s="34" t="s">
         <v>48</v>
@@ -3091,7 +2703,7 @@
       </c>
       <c r="E24" s="36"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" s="34" t="s">
         <v>7</v>
@@ -3104,7 +2716,7 @@
       </c>
       <c r="E25" s="36"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>141</v>
       </c>
@@ -3121,7 +2733,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="9" t="s">
         <v>6</v>
@@ -3134,7 +2746,7 @@
       </c>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>141</v>
       </c>
@@ -3147,7 +2759,7 @@
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="27"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
@@ -3158,7 +2770,7 @@
       </c>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
@@ -3169,7 +2781,7 @@
       </c>
       <c r="E30" s="25"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="27"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
@@ -3182,7 +2794,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24" t="s">
@@ -3195,7 +2807,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
         <v>7</v>
@@ -3208,7 +2820,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="43" t="s">
         <v>48</v>
@@ -3234,16 +2846,16 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3258,7 +2870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -3271,11 +2883,11 @@
       <c r="D2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3288,7 +2900,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>126</v>
       </c>
@@ -3305,7 +2917,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -3318,7 +2930,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -3331,7 +2943,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>122</v>
       </c>
@@ -3344,7 +2956,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3355,7 +2967,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3366,7 +2978,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3377,7 +2989,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3388,7 +3000,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23" t="s">
         <v>5</v>
@@ -3403,7 +3015,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
@@ -3418,7 +3030,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>48</v>
@@ -3431,7 +3043,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -3444,7 +3056,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>48</v>
@@ -3470,16 +3082,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3494,8 +3106,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -3509,8 +3121,8 @@
       </c>
       <c r="E2" s="43"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
       </c>
@@ -3520,9 +3132,9 @@
       <c r="D3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>129</v>
       </c>
@@ -3539,7 +3151,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="11" t="s">
         <v>6</v>
@@ -3552,7 +3164,7 @@
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
         <v>12</v>
@@ -3565,7 +3177,7 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>198</v>
       </c>
@@ -3578,7 +3190,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -3589,7 +3201,7 @@
       </c>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="27"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -3600,7 +3212,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -3611,7 +3223,7 @@
       </c>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -3622,7 +3234,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
@@ -3633,7 +3245,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
       <c r="B13" s="24" t="s">
         <v>5</v>
@@ -3648,7 +3260,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="11" t="s">
         <v>48</v>
@@ -3661,7 +3273,7 @@
       </c>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -3672,8 +3284,8 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="49"/>
       <c r="B16" s="43" t="s">
         <v>48</v>
       </c>
@@ -3683,7 +3295,7 @@
       <c r="D16" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="51"/>
+      <c r="E16" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3699,16 +3311,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3723,7 +3335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3738,7 +3350,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3751,7 +3363,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>122</v>
       </c>
@@ -3768,7 +3380,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -3781,7 +3393,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -3794,7 +3406,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>107</v>
       </c>
@@ -3811,7 +3423,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3822,7 +3434,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3833,7 +3445,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3844,7 +3456,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3855,7 +3467,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -3866,7 +3478,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
@@ -3881,7 +3493,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
         <v>48</v>
@@ -3894,7 +3506,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
         <v>7</v>
@@ -3907,7 +3519,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>48</v>
@@ -3933,16 +3545,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3957,7 +3569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3972,7 +3584,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3985,7 +3597,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>129</v>
       </c>
@@ -4002,7 +3614,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -4015,7 +3627,7 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -4028,7 +3640,7 @@
       </c>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>106</v>
       </c>
@@ -4045,7 +3657,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -4056,7 +3668,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -4067,7 +3679,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -4078,7 +3690,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -4089,7 +3701,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="B12" s="24" t="s">
         <v>5</v>
@@ -4104,7 +3716,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
         <v>48</v>
@@ -4117,7 +3729,7 @@
       </c>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>48</v>
@@ -4130,7 +3742,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -4143,7 +3755,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>48</v>
@@ -4169,16 +3781,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4193,8 +3805,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -4208,8 +3820,8 @@
       </c>
       <c r="E2" s="43"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
       </c>
@@ -4219,9 +3831,9 @@
       <c r="D3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>199</v>
       </c>
@@ -4238,7 +3850,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="11" t="s">
         <v>6</v>
@@ -4251,7 +3863,7 @@
       </c>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
         <v>12</v>
@@ -4264,7 +3876,7 @@
       </c>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>210</v>
       </c>
@@ -4275,11 +3887,11 @@
       <c r="D7" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="56" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -4288,11 +3900,11 @@
       <c r="D8" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="56" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="27"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -4301,11 +3913,11 @@
       <c r="D9" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="56" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -4314,11 +3926,11 @@
       <c r="D10" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="56" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -4327,9 +3939,9 @@
       <c r="D11" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="E11" s="58"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="57"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
@@ -4338,9 +3950,9 @@
       <c r="D12" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="E12" s="58"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="57"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24" t="s">
@@ -4349,11 +3961,11 @@
       <c r="D13" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="57" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
       <c r="B14" s="24"/>
       <c r="C14" s="24" t="s">
@@ -4362,11 +3974,11 @@
       <c r="D14" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="57" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="27"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24" t="s">
@@ -4375,11 +3987,11 @@
       <c r="D15" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="57" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="27"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24" t="s">
@@ -4388,11 +4000,11 @@
       <c r="D16" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="57" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="27"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24" t="s">
@@ -4401,11 +4013,11 @@
       <c r="D17" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="27"/>
       <c r="B18" s="24"/>
       <c r="C18" s="24" t="s">
@@ -4414,11 +4026,11 @@
       <c r="D18" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="E18" s="58" t="s">
+      <c r="E18" s="57" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
       <c r="B19" s="11" t="s">
         <v>48</v>
@@ -4429,9 +4041,9 @@
       <c r="D19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="59"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="58"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="11" t="s">
         <v>7</v>
@@ -4440,10 +4052,10 @@
       <c r="D20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="59"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
+      <c r="E20" s="58"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
       <c r="B21" s="43" t="s">
         <v>48</v>
       </c>
@@ -4453,7 +4065,7 @@
       <c r="D21" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="51"/>
+      <c r="E21" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4465,20 +4077,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345078EF-4E02-4B0D-B586-01D7A19E1A69}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="55.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4493,7 +4105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -4506,11 +4118,11 @@
       <c r="D2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4523,7 +4135,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>282</v>
       </c>
@@ -4540,7 +4152,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -4553,7 +4165,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -4566,7 +4178,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>265</v>
       </c>
@@ -4579,7 +4191,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -4590,7 +4202,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -4601,7 +4213,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -4612,7 +4224,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -4623,7 +4235,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -4634,7 +4246,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>48</v>
@@ -4647,7 +4259,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -4660,7 +4272,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="41"/>
       <c r="B15" s="43" t="s">
         <v>48</v>
@@ -4686,16 +4298,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="92.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4710,7 +4322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -4723,11 +4335,11 @@
       <c r="D2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4740,7 +4352,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>283</v>
       </c>
@@ -4757,7 +4369,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -4770,7 +4382,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -4783,7 +4395,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>271</v>
       </c>
@@ -4796,7 +4408,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -4807,7 +4419,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -4817,10 +4429,10 @@
         <v>279</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -4829,11 +4441,11 @@
       <c r="D10" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="E10" s="57" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="56" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -4844,7 +4456,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>48</v>
@@ -4857,7 +4469,7 @@
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>7</v>
@@ -4870,7 +4482,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
       <c r="B14" s="43" t="s">
         <v>48</v>

</xml_diff>